<commit_message>
better layout for analog buffers
</commit_message>
<xml_diff>
--- a/STM32F407 era/Traction control modul/sensor overview.xlsx
+++ b/STM32F407 era/Traction control modul/sensor overview.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>sensor</t>
   </si>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,6 +339,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -374,6 +391,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kontor">
@@ -529,13 +563,13 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.375" customWidth="1"/>
+    <col min="2" max="2" width="9.625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
@@ -856,6 +890,9 @@
       <c r="H12">
         <v>0</v>
       </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -904,6 +941,9 @@
       <c r="H14">
         <v>0</v>
       </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -928,6 +968,9 @@
       <c r="H15">
         <v>0</v>
       </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -976,6 +1019,9 @@
       <c r="H17">
         <v>0</v>
       </c>
+      <c r="J17" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -999,6 +1045,9 @@
       </c>
       <c r="H18">
         <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>